<commit_message>
added reading rear_geo from an excel file
</commit_message>
<xml_diff>
--- a/numbers1.xlsx
+++ b/numbers1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaveh\OneDrive\Documents\GitHub\Mechanical_Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02034821-E38A-4925-93E3-64FE1AEBB832}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218A2571-6B50-4261-83AF-26920F766625}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
   <si>
     <t>Value(x)</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Forces: 3G Bump, 1G Turn (to the right) , 1G Brake</t>
-  </si>
-  <si>
-    <t>Rear Suspension</t>
   </si>
 </sst>
 </file>
@@ -749,7 +746,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,17 +1273,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC4DD83-EB2C-481D-8086-B3316FCB5B0F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
+      <c r="A1">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.4699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.18759999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.9369999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.27939999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.27939999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.2739999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.88319999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>